<commit_message>
changed meta template example
</commit_message>
<xml_diff>
--- a/resources/datalineage/example_input/meta_template.xlsx
+++ b/resources/datalineage/example_input/meta_template.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacbeekers/gitrepos/metadata-registry-interface-specifications/resources/datalineage/example_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56769B74-C4ED-6843-B9B7-23CAD11EB89F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1067F77F-6399-AA44-8512-A60F26DF7791}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="50060" windowHeight="28300" xr2:uid="{72BBAAF7-540E-4135-A93E-007AAACCE38C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="50060" windowHeight="28300" activeTab="1" xr2:uid="{72BBAAF7-540E-4135-A93E-007AAACCE38C}"/>
   </bookViews>
   <sheets>
-    <sheet name="excel format" sheetId="1" r:id="rId1"/>
-    <sheet name="glossary" sheetId="3" r:id="rId2"/>
+    <sheet name="Datasets" sheetId="6" r:id="rId1"/>
+    <sheet name="DataElements" sheetId="1" r:id="rId2"/>
+    <sheet name="glossary" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'excel format'!$A$1:$AF$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DataElements!$A$1:$L$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Datasets!$A$1:$U$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,10 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="109">
-  <si>
-    <t>Dataset</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="110">
   <si>
     <t>datasetdesc</t>
   </si>
@@ -172,9 +171,6 @@
     <t>datasource_id</t>
   </si>
   <si>
-    <t>data_layer</t>
-  </si>
-  <si>
     <t>src_technical_system</t>
   </si>
   <si>
@@ -223,9 +219,6 @@
     <t>physical_model_zone</t>
   </si>
   <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
     <t>Customer</t>
   </si>
   <si>
@@ -235,9 +228,6 @@
     <t>UID</t>
   </si>
   <si>
-    <t>String</t>
-  </si>
-  <si>
     <t>tgt_path</t>
   </si>
   <si>
@@ -328,12 +318,6 @@
     <t>Nick name</t>
   </si>
   <si>
-    <t>Mapping_Dataset_or_DataElement</t>
-  </si>
-  <si>
-    <t>DataElement</t>
-  </si>
-  <si>
     <t>JBE.APP.2634</t>
   </si>
   <si>
@@ -365,6 +349,27 @@
   </si>
   <si>
     <t>Contains the employee data in our data model</t>
+  </si>
+  <si>
+    <t>dataset_ref</t>
+  </si>
+  <si>
+    <t>src_layer</t>
+  </si>
+  <si>
+    <t>INITALS</t>
+  </si>
+  <si>
+    <t>Synapse</t>
+  </si>
+  <si>
+    <t>Internal Employees</t>
+  </si>
+  <si>
+    <t>Dutch Customers</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -585,10 +590,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -887,382 +888,502 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE3E65B-C8B6-FE43-81D3-E7F6AAD85456}">
+  <dimension ref="A1:U3"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="17" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.1640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="48" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.33203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="1" t="str">
+        <f>_xlfn.CONCAT(D2,"/",E2,"/",F2,"/",G2)</f>
+        <v>acquisition_layer/transient_zone/Mainframe/CUST</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="O2" s="1" t="str">
+        <f>_xlfn.CONCAT(L2,"/",M2,"/",N2)</f>
+        <v>integration_layer/physical_model_zone/1.2.0</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="1" t="str">
+        <f>_xlfn.CONCAT(D3,"/",E3,"/",F3,"/",G3)</f>
+        <v>acquisition_layer/transient_zone/EDL/EMP</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="O3" s="1" t="str">
+        <f>_xlfn.CONCAT(L3,"/",M3,"/",N3)</f>
+        <v>integration_layer/physical_model_zone/1.2.0</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:U5" xr:uid="{FEF3A2B1-0E0B-B444-A1BE-36A58D419FE0}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63869BB-5BCD-4EEC-8C31-2EAA5543C529}">
-  <dimension ref="A1:AF11"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="27.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="48" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="31.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.6640625" style="1" customWidth="1"/>
-    <col min="14" max="15" width="17" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.33203125" style="1" customWidth="1"/>
-    <col min="17" max="20" width="17" style="1" customWidth="1"/>
-    <col min="21" max="21" width="32.5" style="1" customWidth="1"/>
-    <col min="22" max="22" width="36.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="34.1640625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="48" style="1" customWidth="1"/>
-    <col min="25" max="25" width="28.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="17" style="1" customWidth="1"/>
-    <col min="30" max="30" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="48" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q1" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="R1" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="U1" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="V1" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="W1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="X1" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z1" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB1" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="AD1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE1" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="AF1" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="1" t="str">
-        <f>_xlfn.CONCAT(D2,"/",E2,"/",F2,"/",G2)</f>
-        <v>acquisition_layer/transient_zone/Mainframe/CUST</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="9"/>
-      <c r="S2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="U2" s="1" t="s">
+      <c r="D6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="V2" s="1" t="str">
-        <f>_xlfn.CONCAT(S2,"/",T2,"/",U2)</f>
-        <v>integration_layer/physical_model_zone/1.0.0</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="K3" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="L3" s="9" t="s">
+      <c r="J8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>2</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="K4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="K5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="K6" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="K7" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="K8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="D9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H9" s="1" t="str">
-        <f>_xlfn.CONCAT(D9,"/",E9,"/",F9,"/",G9)</f>
-        <v>acquisition_layer/transient_zone/EDL/EMP</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="V9" s="1" t="str">
-        <f>_xlfn.CONCAT(S9,"/",T9,"/",U9)</f>
-        <v>integration_layer/physical_model_zone/1.2.0</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z10" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AF8" xr:uid="{DBEF8181-D3DC-594B-ABC0-7F6ADEFFC51B}"/>
+  <autoFilter ref="A1:L7" xr:uid="{DBEF8181-D3DC-594B-ABC0-7F6ADEFFC51B}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218933E6-5796-4784-85A7-374FC732FEC3}">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -1280,240 +1401,240 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="C1" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="F2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="F3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C4" s="1"/>
       <c r="F4" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="1"/>
     </row>

</xml_diff>